<commit_message>
categorization merged into main dataframe. data collection, transformation & categorization done!
</commit_message>
<xml_diff>
--- a/manually_edited_data/interest_groups_categories.xlsx
+++ b/manually_edited_data/interest_groups_categories.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,526 +568,478 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>458348124803-65</t>
+          <t>070028236358-54</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Skeleton Technologies OÜ (SKL)</t>
+          <t>ASML Netherlands B.V. (ASML)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>070028236358-54</t>
+          <t>89093924456-06</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ASML Netherlands B.V. (ASML)</t>
+          <t>Vereinigung der österreichischen Industrie - Industriellenvereinigung (IV)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>89093924456-06</t>
+          <t>27762251795-15</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Vereinigung der österreichischen Industrie - Industriellenvereinigung (IV)</t>
+          <t>Confederazione Generale dell'Industria Italiana (Confindustria)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>27762251795-15</t>
+          <t>142903829084-58</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Confederazione Generale dell'Industria Italiana (Confindustria)</t>
+          <t>Stiftung Neue Verantwortung e.V. (SNV)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>142903829084-58</t>
+          <t>001968511387-52</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Stiftung Neue Verantwortung e.V. (SNV)</t>
+          <t>European Internet Forum (EIF)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>001968511387-52</t>
+          <t>1771817758-48</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>European Internet Forum (EIF)</t>
+          <t>Bundesverband der Deutschen Industrie e.V. (BDI)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1771817758-48</t>
+          <t>475891045627-85</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Bundesverband der Deutschen Industrie e.V. (BDI)</t>
+          <t>AT &amp; S AUSTRIA TECHNOLOGIE &amp; SYSTEMTECHNIK AKTIENGESELLSCHAFT</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>475891045627-85</t>
+          <t>336735239719-29</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>AT &amp; S AUSTRIA TECHNOLOGIE &amp; SYSTEMTECHNIK AKTIENGESELLSCHAFT</t>
+          <t>Kalray SA</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>336735239719-29</t>
+          <t>986044541551-20</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Kalray SA</t>
+          <t>Stellantis</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>986044541551-20</t>
+          <t>8999533555-91</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Stellantis</t>
+          <t>Robert Bosch GmbH</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>8999533555-91</t>
+          <t>04201463642-88</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Robert Bosch GmbH</t>
+          <t>APPLiA (Home Appliance Europe) (APPLiA)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>04201463642-88</t>
+          <t>21856815315-64</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>APPLiA (Home Appliance Europe) (APPLiA)</t>
+          <t>EUROSMART</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>21856815315-64</t>
+          <t>35124436517-75</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>EUROSMART</t>
+          <t>Fraunhofer-Gesellschaft (FhG)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>35124436517-75</t>
+          <t>898711618618-45</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Fraunhofer-Gesellschaft (FhG)</t>
+          <t>NXP Semiconductors Netherlands B.V. (NXP)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>898711618618-45</t>
+          <t>588327811384-96</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>NXP Semiconductors Netherlands B.V. (NXP)</t>
+          <t>Apple Inc.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>588327811384-96</t>
+          <t>721066539792-75</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Apple Inc.</t>
+          <t>GLOBALFOUNDRIES Management Services Limited Liability Company &amp; Co. KG (GF Dresden)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>721066539792-75</t>
+          <t>7721359944-96</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>GLOBALFOUNDRIES Management Services Limited Liability Company &amp; Co. KG (GF Dresden)</t>
+          <t>IBM Corporation (IBM)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>7721359944-96</t>
+          <t>40471017282-57</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>IBM Corporation (IBM)</t>
+          <t>Samsung Electronics Europe</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>40471017282-57</t>
+          <t>266271142555-68</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Samsung Electronics Europe</t>
+          <t>Taiwan Semiconductor Manufacturing Company Ltd (TSMC)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>266271142555-68</t>
+          <t>3305029916-47</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Taiwan Semiconductor Manufacturing Company Ltd (TSMC)</t>
+          <t>Scania AB (publ) (Scania)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>3305029916-47</t>
+          <t>10751968675-85</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Scania AB (publ) (Scania)</t>
+          <t>Infineon Technologies AG</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>10751968675-85</t>
+          <t>532086816465-17</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Infineon Technologies AG</t>
+          <t>Arm Holdings</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>532086816465-17</t>
+          <t>22400601191-42</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Arm Holdings</t>
+          <t>Deutscher Industrie- und Handelskammertag e.V. (DIHK)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>22400601191-42</t>
+          <t>764184537594-67</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Deutscher Industrie- und Handelskammertag e.V. (DIHK)</t>
+          <t>SAFRAN</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>94857385769-70</t>
+          <t>174684235534-60</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>AIR LIQUIDE (AIR LIQUIDE)</t>
+          <t>Qualcomm Communications SARL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>90947457424-20</t>
+          <t>64270747023-20</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ENGIE (ENGIE)</t>
+          <t>DIGITALEUROPE (DE)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>764184537594-67</t>
+          <t>20210641335-88</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SAFRAN</t>
+          <t>ORGALIME – The European Technology Industries (ORGALIME)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>174684235534-60</t>
+          <t>5749958415-41</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Qualcomm Communications SARL</t>
+          <t>Confederation of Danish Industry (DI)</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>284336314886-25</t>
+          <t>865956522785-09</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Snam S.p.A. (Snam S.p.A.)</t>
+          <t>Fraunhofer Austria Reserach GmbH (FhA)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>64270747023-20</t>
+          <t>248908039789-74</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>DIGITALEUROPE (DE)</t>
+          <t>Melexis NV</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20210641335-88</t>
+          <t>367850645092-18</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ORGALIME – The European Technology Industries (ORGALIME)</t>
+          <t>Nordic Semiconductor ASA</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5749958415-41</t>
+          <t>030658245107-49</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Confederation of Danish Industry (DI)</t>
+          <t>Alcyon Photonics SL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>865956522785-09</t>
+          <t>041592911733-05</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Fraunhofer Austria Reserach GmbH (FhA)</t>
+          <t>Centre on Regulation in Europe (CERRE)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>248908039789-74</t>
+          <t>71635694112-37</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Melexis NV</t>
+          <t>FEANI (FEANI)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>367850645092-18</t>
+          <t>147656111703-83</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Nordic Semiconductor ASA</t>
+          <t>European Forum of technical and Vocational Education and Training (EfVET)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>030658245107-49</t>
+          <t>358284014848-82</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Alcyon Photonics SL</t>
+          <t>industriAll European Trade Union (industriAll)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>041592911733-05</t>
+          <t>52774696782-43</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Centre on Regulation in Europe (CERRE)</t>
+          <t>Commissariat à l'Energie atomique et aux énergies alternatives (CEA)</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>71635694112-37</t>
+          <t>817789336491-32</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>FEANI (FEANI)</t>
+          <t>SOITEC (SOITEC)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>147656111703-83</t>
+          <t>402302029423-14</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>European Forum of technical and Vocational Education and Training (EfVET)</t>
+          <t>SEMI Europe (SEMI)</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>358284014848-82</t>
+          <t>243961945295-86</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
-        <is>
-          <t>industriAll European Trade Union (industriAll)</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>52774696782-43</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Commissariat à l'Energie atomique et aux énergies alternatives (CEA)</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>817789336491-32</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>SOITEC (SOITEC)</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>402302029423-14</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>SEMI Europe (SEMI)</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>243961945295-86</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
         <is>
           <t>SOITEC</t>
         </is>

</xml_diff>

<commit_message>
switched to CSV for final export. Changed time period and categorized additional interest groups
</commit_message>
<xml_diff>
--- a/manually_edited_data/interest_groups_categories.xlsx
+++ b/manually_edited_data/interest_groups_categories.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,598 +448,670 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>236869539281-13</t>
+          <t>070028236358-54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The LEGO Group</t>
+          <t>ASML Netherlands B.V. (ASML)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>97921387213-35</t>
+          <t>583393138546-76</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Interuniversitair Micro-Electronica Centrum (IMEC)</t>
+          <t>Applied Materials (AMAT)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>70843878143-13</t>
+          <t>97921387213-35</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>STMicroelectronics (ST)</t>
+          <t>Interuniversitair Micro-Electronica Centrum (IMEC)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>00358442856-45</t>
+          <t>866541247974-60</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>QUALCOMM Inc. (QCOM (NASDAQ))</t>
+          <t>NVIDIA Corporation</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>7459401905-60</t>
+          <t>00358442856-45</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Intel Corporation</t>
+          <t>QUALCOMM Inc. (QCOM (NASDAQ))</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>012717123539-58</t>
+          <t>389630949944-21</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>European Chamber of Commerce Taiwan (ECCT)</t>
+          <t>ARDIAN France</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>494613715191-85</t>
+          <t>236569017571-35</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cisco Systems Inc. (Cisco)</t>
+          <t>Association Nationale des Sociétés par Actions (ANSA)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>524976815651-12</t>
+          <t>7459401905-60</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Centre for European Reform (CER)</t>
+          <t>Intel Corporation</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>194094423131-36</t>
+          <t>809121549545-61</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ZF Friedrichshafen AG</t>
+          <t>Taiwan Semiconductor Manufacturing Company Ltd</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>547225616323-13</t>
+          <t>236869539281-13</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Tesla, Inc. (Tesla)</t>
+          <t>The LEGO Group</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>070028236358-54</t>
+          <t>70843878143-13</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ASML Netherlands B.V. (ASML)</t>
+          <t>STMicroelectronics (ST)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>89093924456-06</t>
+          <t>012717123539-58</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Vereinigung der österreichischen Industrie - Industriellenvereinigung (IV)</t>
+          <t>European Chamber of Commerce Taiwan (ECCT)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>27762251795-15</t>
+          <t>494613715191-85</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Confederazione Generale dell'Industria Italiana (Confindustria)</t>
+          <t>Cisco Systems Inc. (Cisco)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>142903829084-58</t>
+          <t>524976815651-12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Stiftung Neue Verantwortung e.V. (SNV)</t>
+          <t>Centre for European Reform (CER)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>001968511387-52</t>
+          <t>194094423131-36</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>European Internet Forum (EIF)</t>
+          <t>ZF Friedrichshafen AG</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1771817758-48</t>
+          <t>547225616323-13</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Bundesverband der Deutschen Industrie e.V. (BDI)</t>
+          <t>Tesla, Inc. (Tesla)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>475891045627-85</t>
+          <t>89093924456-06</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>AT &amp; S AUSTRIA TECHNOLOGIE &amp; SYSTEMTECHNIK AKTIENGESELLSCHAFT</t>
+          <t>Vereinigung der österreichischen Industrie - Industriellenvereinigung (IV)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>336735239719-29</t>
+          <t>27762251795-15</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Kalray SA</t>
+          <t>Confederazione Generale dell'Industria Italiana (Confindustria)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>986044541551-20</t>
+          <t>142903829084-58</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Stellantis</t>
+          <t>Stiftung Neue Verantwortung e.V. (SNV)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>8999533555-91</t>
+          <t>001968511387-52</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Robert Bosch GmbH</t>
+          <t>European Internet Forum (EIF)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04201463642-88</t>
+          <t>1771817758-48</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>APPLiA (Home Appliance Europe) (APPLiA)</t>
+          <t>Bundesverband der Deutschen Industrie e.V. (BDI)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>21856815315-64</t>
+          <t>475891045627-85</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>EUROSMART</t>
+          <t>AT &amp; S AUSTRIA TECHNOLOGIE &amp; SYSTEMTECHNIK AKTIENGESELLSCHAFT</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>35124436517-75</t>
+          <t>336735239719-29</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Fraunhofer-Gesellschaft (FhG)</t>
+          <t>Kalray SA</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>898711618618-45</t>
+          <t>986044541551-20</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>NXP Semiconductors Netherlands B.V. (NXP)</t>
+          <t>Stellantis</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>588327811384-96</t>
+          <t>8999533555-91</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Apple Inc.</t>
+          <t>Robert Bosch GmbH</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>721066539792-75</t>
+          <t>04201463642-88</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>GLOBALFOUNDRIES Management Services Limited Liability Company &amp; Co. KG (GF Dresden)</t>
+          <t>APPLiA (Home Appliance Europe) (APPLiA)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>7721359944-96</t>
+          <t>21856815315-64</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>IBM Corporation (IBM)</t>
+          <t>EUROSMART</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>40471017282-57</t>
+          <t>35124436517-75</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Samsung Electronics Europe</t>
+          <t>Fraunhofer-Gesellschaft (FhG)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>266271142555-68</t>
+          <t>898711618618-45</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Taiwan Semiconductor Manufacturing Company Ltd (TSMC)</t>
+          <t>NXP Semiconductors Netherlands B.V. (NXP)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>3305029916-47</t>
+          <t>588327811384-96</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Scania AB (publ) (Scania)</t>
+          <t>Apple Inc.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>10751968675-85</t>
+          <t>721066539792-75</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Infineon Technologies AG</t>
+          <t>GLOBALFOUNDRIES Management Services Limited Liability Company &amp; Co. KG (GF Dresden)</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>532086816465-17</t>
+          <t>7721359944-96</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Arm Holdings</t>
+          <t>IBM Corporation (IBM)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>22400601191-42</t>
+          <t>40471017282-57</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Deutscher Industrie- und Handelskammertag e.V. (DIHK)</t>
+          <t>Samsung Electronics Europe</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>764184537594-67</t>
+          <t>266271142555-68</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SAFRAN</t>
+          <t>Taiwan Semiconductor Manufacturing Company Ltd (TSMC)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>174684235534-60</t>
+          <t>3305029916-47</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Qualcomm Communications SARL</t>
+          <t>Scania AB (publ) (Scania)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>64270747023-20</t>
+          <t>10751968675-85</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>DIGITALEUROPE (DE)</t>
+          <t>Infineon Technologies AG</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20210641335-88</t>
+          <t>532086816465-17</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ORGALIME – The European Technology Industries (ORGALIME)</t>
+          <t>Arm Holdings</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5749958415-41</t>
+          <t>789826549861-77</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Confederation of Danish Industry (DI)</t>
+          <t>Synopsys Inc.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>865956522785-09</t>
+          <t>22400601191-42</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Fraunhofer Austria Reserach GmbH (FhA)</t>
+          <t>Deutscher Industrie- und Handelskammertag e.V. (DIHK)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>248908039789-74</t>
+          <t>764184537594-67</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Melexis NV</t>
+          <t>SAFRAN</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>367850645092-18</t>
+          <t>174684235534-60</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Nordic Semiconductor ASA</t>
+          <t>Qualcomm Communications SARL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>030658245107-49</t>
+          <t>64270747023-20</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Alcyon Photonics SL</t>
+          <t>DIGITALEUROPE (DE)</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>041592911733-05</t>
+          <t>20210641335-88</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Centre on Regulation in Europe (CERRE)</t>
+          <t>ORGALIME – The European Technology Industries (ORGALIME)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>71635694112-37</t>
+          <t>5749958415-41</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>FEANI (FEANI)</t>
+          <t>Confederation of Danish Industry (DI)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>147656111703-83</t>
+          <t>865956522785-09</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>European Forum of technical and Vocational Education and Training (EfVET)</t>
+          <t>Fraunhofer Austria Reserach GmbH (FhA)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>358284014848-82</t>
+          <t>248908039789-74</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>industriAll European Trade Union (industriAll)</t>
+          <t>Melexis NV</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>52774696782-43</t>
+          <t>367850645092-18</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Commissariat à l'Energie atomique et aux énergies alternatives (CEA)</t>
+          <t>Nordic Semiconductor ASA</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>817789336491-32</t>
+          <t>030658245107-49</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SOITEC (SOITEC)</t>
+          <t>Alcyon Photonics SL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>402302029423-14</t>
+          <t>041592911733-05</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SEMI Europe (SEMI)</t>
+          <t>Centre on Regulation in Europe (CERRE)</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>71635694112-37</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>FEANI (FEANI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>147656111703-83</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>European Forum of technical and Vocational Education and Training (EfVET)</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>358284014848-82</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>industriAll European Trade Union (industriAll)</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>52774696782-43</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Commissariat à l'Energie atomique et aux énergies alternatives (CEA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>817789336491-32</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>SOITEC (SOITEC)</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>402302029423-14</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>SEMI Europe (SEMI)</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
           <t>243961945295-86</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B57" t="inlineStr">
         <is>
           <t>SOITEC</t>
         </is>

</xml_diff>